<commit_message>
Get theme and non-theme rows consistent in the test file
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1694889 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/Themes2.xlsx
+++ b/test-data/spreadsheet/Themes2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>dk1</t>
   </si>
@@ -107,13 +107,19 @@
   </si>
   <si>
     <t>std green</t>
+  </si>
+  <si>
+    <t>Dark Blue</t>
+  </si>
+  <si>
+    <t>dark blue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,8 +262,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +319,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -319,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -348,11 +367,43 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -374,237 +425,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -916,7 +736,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -946,6 +766,18 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
@@ -961,41 +793,38 @@
         <v>22</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>23</v>
+      <c r="B4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>24</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1072,29 +901,25 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G3:G5 G7">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5 G7">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"std red"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>"std green"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G4">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>2</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"std green"</formula>
+      <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>